<commit_message>
Change to similar to old site.
</commit_message>
<xml_diff>
--- a/markdown_generator/publications.xlsx
+++ b/markdown_generator/publications.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/markcartwright/git/minimal-mistakes/markdown_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F36D9C51-25ED-514D-97FB-02A9F1B8FC42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30264C76-FF47-0C4D-B5C1-0BFEF5283F9D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1600" yWindow="2660" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="1600" yWindow="2660" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publications" sheetId="1" r:id="rId1"/>
@@ -712,9 +712,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -1202,11 +1202,12 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1562,11 +1563,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1675,7 +1676,7 @@
         <v>15</v>
       </c>
       <c r="I3">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="K3" t="s">
         <v>16</v>
@@ -1716,7 +1717,7 @@
         <v>213</v>
       </c>
       <c r="I4">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="L4" t="s">
         <v>24</v>
@@ -1835,7 +1836,7 @@
         <v>213</v>
       </c>
       <c r="I8">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="Q8" t="s">
         <v>205</v>
@@ -1983,7 +1984,7 @@
         <v>213</v>
       </c>
       <c r="I13">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K13" t="s">
         <v>158</v>
@@ -2093,8 +2094,8 @@
       <c r="G16" t="s">
         <v>164</v>
       </c>
-      <c r="I16">
-        <v>33</v>
+      <c r="I16" s="4">
+        <v>50</v>
       </c>
       <c r="M16" s="1" t="s">
         <v>165</v>
@@ -2207,7 +2208,7 @@
         <v>213</v>
       </c>
       <c r="I20">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="K20" t="s">
         <v>170</v>
@@ -2563,7 +2564,7 @@
         <v>213</v>
       </c>
       <c r="I33">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="O33" s="1" t="s">
         <v>188</v>
@@ -2600,14 +2601,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="M13" r:id="rId1"/>
-    <hyperlink ref="O15" r:id="rId2"/>
-    <hyperlink ref="M15" r:id="rId3"/>
-    <hyperlink ref="M16" r:id="rId4"/>
-    <hyperlink ref="O16" r:id="rId5"/>
-    <hyperlink ref="M20" r:id="rId6"/>
-    <hyperlink ref="O22" r:id="rId7"/>
-    <hyperlink ref="O33" r:id="rId8"/>
+    <hyperlink ref="M13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="O15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="M15" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="M16" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="O16" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="M20" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="O22" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="O33" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>